<commit_message>
Initial commit for my image vercel converter app 5
</commit_message>
<xml_diff>
--- a/uploads/img.xlsx
+++ b/uploads/img.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsidd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{084E3398-872C-47AE-A305-186C803F629B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B4F06A1-3E36-4D0A-89AD-83BD1D39FA5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{A1BC502E-D052-42BE-AF07-F472BED51F8E}"/>
   </bookViews>
@@ -36,7 +36,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
   <si>
     <t>name</t>
   </si>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0FC1954-0DDF-4B34-81E7-6F50B0A3734E}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,28 +464,31 @@
     <col min="2" max="2" width="43.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>